<commit_message>
Added PLS regression and results.
</commit_message>
<xml_diff>
--- a/data/spx/spx.xlsx
+++ b/data/spx/spx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\claud\Desktop\dm\bb-llm-sentiment\data\spx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3F353AA-D50A-44CD-820F-99475064F848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8732A5D-782A-40F5-8549-ED203DAA56D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{2C4A662B-7109-4E2A-B337-75408B2E0E60}"/>
   </bookViews>
@@ -426,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8517D59-D0C8-4CAF-AA06-A662775BA6E5}">
-  <dimension ref="A1:B2775"/>
+  <dimension ref="A1:D2775"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A1268" workbookViewId="0">
+      <selection activeCell="A1281" sqref="A1281"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4014,7 +4014,7 @@
         <v>4602.45</v>
       </c>
     </row>
-    <row r="449" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="449" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A449" s="2">
         <v>44649</v>
       </c>
@@ -4022,7 +4022,7 @@
         <v>4631.6000000000004</v>
       </c>
     </row>
-    <row r="450" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="450" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A450" s="2">
         <v>44648</v>
       </c>
@@ -4030,7 +4030,7 @@
         <v>4575.5200000000004</v>
       </c>
     </row>
-    <row r="451" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="451" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A451" s="2">
         <v>44645</v>
       </c>
@@ -4038,7 +4038,7 @@
         <v>4543.0600000000004</v>
       </c>
     </row>
-    <row r="452" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="452" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A452" s="2">
         <v>44644</v>
       </c>
@@ -4046,7 +4046,7 @@
         <v>4520.16</v>
       </c>
     </row>
-    <row r="453" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="453" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A453" s="2">
         <v>44643</v>
       </c>
@@ -4054,127 +4054,188 @@
         <v>4456.24</v>
       </c>
     </row>
-    <row r="454" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="454" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A454" s="2">
         <v>44642</v>
       </c>
       <c r="B454">
         <v>4511.6099999999997</v>
       </c>
-    </row>
-    <row r="455" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C454">
+        <v>14</v>
+      </c>
+      <c r="D454">
+        <f>(B454-$B$468)/$B$468</f>
+        <v>2.8512221477519802E-2</v>
+      </c>
+    </row>
+    <row r="455" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A455" s="2">
         <v>44641</v>
       </c>
       <c r="B455">
         <v>4461.18</v>
       </c>
-    </row>
-    <row r="456" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C455">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="456" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A456" s="2">
         <v>44638</v>
       </c>
       <c r="B456">
         <v>4463.12</v>
       </c>
-    </row>
-    <row r="457" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C456">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="457" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A457" s="2">
         <v>44637</v>
       </c>
       <c r="B457">
         <v>4411.67</v>
       </c>
-    </row>
-    <row r="458" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C457">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="458" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A458" s="2">
         <v>44636</v>
       </c>
       <c r="B458">
         <v>4357.8599999999997</v>
       </c>
-    </row>
-    <row r="459" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C458">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="459" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A459" s="2">
         <v>44635</v>
       </c>
       <c r="B459">
         <v>4262.45</v>
       </c>
-    </row>
-    <row r="460" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C459">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="460" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A460" s="2">
         <v>44634</v>
       </c>
       <c r="B460">
         <v>4173.1099999999997</v>
       </c>
-    </row>
-    <row r="461" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C460">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="461" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A461" s="2">
         <v>44631</v>
       </c>
       <c r="B461">
         <v>4204.3100000000004</v>
       </c>
-    </row>
-    <row r="462" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C461">
+        <v>7</v>
+      </c>
+      <c r="D461">
+        <f>(B461-$B$468)/$B$468</f>
+        <v>-4.1542992882773112E-2</v>
+      </c>
+    </row>
+    <row r="462" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A462" s="2">
         <v>44630</v>
       </c>
       <c r="B462">
         <v>4259.5200000000004</v>
       </c>
-    </row>
-    <row r="463" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C462">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="463" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A463" s="2">
         <v>44629</v>
       </c>
       <c r="B463">
         <v>4277.88</v>
       </c>
-    </row>
-    <row r="464" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C463">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="464" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A464" s="2">
         <v>44628</v>
       </c>
       <c r="B464">
         <v>4170.7</v>
       </c>
-    </row>
-    <row r="465" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C464">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="465" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A465" s="2">
         <v>44627</v>
       </c>
       <c r="B465">
         <v>4201.09</v>
       </c>
-    </row>
-    <row r="466" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C465">
+        <v>3</v>
+      </c>
+      <c r="D465">
+        <f>(B465-$B$468)/$B$468</f>
+        <v>-4.2277056632334324E-2</v>
+      </c>
+    </row>
+    <row r="466" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A466" s="2">
         <v>44624</v>
       </c>
       <c r="B466">
         <v>4328.87</v>
       </c>
-    </row>
-    <row r="467" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C466">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="467" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A467" s="2">
         <v>44623</v>
       </c>
       <c r="B467">
         <v>4363.49</v>
       </c>
-    </row>
-    <row r="468" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C467">
+        <v>1</v>
+      </c>
+      <c r="D467">
+        <f>(B467-$B$468)/$B$468</f>
+        <v>-5.2547110022934211E-3</v>
+      </c>
+    </row>
+    <row r="468" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A468" s="2">
         <v>44622</v>
       </c>
       <c r="B468">
         <v>4386.54</v>
       </c>
-    </row>
-    <row r="469" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C468">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="469" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A469" s="2">
         <v>44621</v>
       </c>
@@ -4182,7 +4243,7 @@
         <v>4306.26</v>
       </c>
     </row>
-    <row r="470" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="470" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A470" s="2">
         <v>44620</v>
       </c>
@@ -4190,7 +4251,7 @@
         <v>4373.9399999999996</v>
       </c>
     </row>
-    <row r="471" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="471" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A471" s="2">
         <v>44617</v>
       </c>
@@ -4198,7 +4259,7 @@
         <v>4384.6499999999996</v>
       </c>
     </row>
-    <row r="472" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="472" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A472" s="2">
         <v>44616</v>
       </c>
@@ -4206,7 +4267,7 @@
         <v>4288.7</v>
       </c>
     </row>
-    <row r="473" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="473" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A473" s="2">
         <v>44615</v>
       </c>
@@ -4214,7 +4275,7 @@
         <v>4225.5</v>
       </c>
     </row>
-    <row r="474" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="474" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A474" s="2">
         <v>44614</v>
       </c>
@@ -4222,7 +4283,7 @@
         <v>4304.76</v>
       </c>
     </row>
-    <row r="475" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="475" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A475" s="2">
         <v>44610</v>
       </c>
@@ -4230,7 +4291,7 @@
         <v>4348.87</v>
       </c>
     </row>
-    <row r="476" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="476" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A476" s="2">
         <v>44609</v>
       </c>
@@ -4238,7 +4299,7 @@
         <v>4380.26</v>
       </c>
     </row>
-    <row r="477" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="477" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A477" s="2">
         <v>44608</v>
       </c>
@@ -4246,7 +4307,7 @@
         <v>4475.01</v>
       </c>
     </row>
-    <row r="478" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="478" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A478" s="2">
         <v>44607</v>
       </c>
@@ -4254,7 +4315,7 @@
         <v>4471.07</v>
       </c>
     </row>
-    <row r="479" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="479" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A479" s="2">
         <v>44606</v>
       </c>
@@ -4262,7 +4323,7 @@
         <v>4401.67</v>
       </c>
     </row>
-    <row r="480" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="480" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A480" s="2">
         <v>44603</v>
       </c>
@@ -10542,7 +10603,7 @@
         <v>2447.89</v>
       </c>
     </row>
-    <row r="1265" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1265" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1265" s="2">
         <v>43467</v>
       </c>
@@ -10550,7 +10611,7 @@
         <v>2510.0300000000002</v>
       </c>
     </row>
-    <row r="1266" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1266" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1266" s="2">
         <v>43465</v>
       </c>
@@ -10558,7 +10619,7 @@
         <v>2506.85</v>
       </c>
     </row>
-    <row r="1267" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1267" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1267" s="2">
         <v>43462</v>
       </c>
@@ -10566,127 +10627,188 @@
         <v>2485.7399999999998</v>
       </c>
     </row>
-    <row r="1268" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1268" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1268" s="2">
         <v>43461</v>
       </c>
       <c r="B1268">
         <v>2488.83</v>
       </c>
-    </row>
-    <row r="1269" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1268">
+        <v>14</v>
+      </c>
+      <c r="D1268">
+        <f>(B1268-$B$1282)/$B$1282</f>
+        <v>-7.6826350637066679E-2</v>
+      </c>
+    </row>
+    <row r="1269" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1269" s="2">
         <v>43460</v>
       </c>
       <c r="B1269">
         <v>2467.6999999999998</v>
       </c>
-    </row>
-    <row r="1270" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1269">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1270" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1270" s="2">
         <v>43458</v>
       </c>
       <c r="B1270">
         <v>2351.1</v>
       </c>
-    </row>
-    <row r="1271" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1270">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1271" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1271" s="2">
         <v>43455</v>
       </c>
       <c r="B1271">
         <v>2416.62</v>
       </c>
-    </row>
-    <row r="1272" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1271">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1272" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1272" s="2">
         <v>43454</v>
       </c>
       <c r="B1272">
         <v>2467.42</v>
       </c>
-    </row>
-    <row r="1273" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1272">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1273" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1273" s="2">
         <v>43453</v>
       </c>
       <c r="B1273">
         <v>2506.96</v>
       </c>
-    </row>
-    <row r="1274" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1273">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1274" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1274" s="2">
         <v>43452</v>
       </c>
       <c r="B1274">
         <v>2546.16</v>
       </c>
-    </row>
-    <row r="1275" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1274">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1275" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1275" s="2">
         <v>43451</v>
       </c>
       <c r="B1275">
         <v>2545.94</v>
       </c>
-    </row>
-    <row r="1276" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1275">
+        <v>7</v>
+      </c>
+      <c r="D1275">
+        <f>(B1275-$B$1282)/$B$1282</f>
+        <v>-5.5642723344275592E-2</v>
+      </c>
+    </row>
+    <row r="1276" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1276" s="2">
         <v>43448</v>
       </c>
       <c r="B1276">
         <v>2599.9499999999998</v>
       </c>
-    </row>
-    <row r="1277" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1276">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1277" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1277" s="2">
         <v>43447</v>
       </c>
       <c r="B1277">
         <v>2650.54</v>
       </c>
-    </row>
-    <row r="1278" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1277">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1278" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1278" s="2">
         <v>43446</v>
       </c>
       <c r="B1278">
         <v>2651.07</v>
       </c>
-    </row>
-    <row r="1279" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1278">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1279" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1279" s="2">
         <v>43445</v>
       </c>
       <c r="B1279">
         <v>2636.78</v>
       </c>
-    </row>
-    <row r="1280" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1279">
+        <v>3</v>
+      </c>
+      <c r="D1279">
+        <f>(B1279-$B$1282)/$B$1282</f>
+        <v>-2.194773641944384E-2</v>
+      </c>
+    </row>
+    <row r="1280" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1280" s="2">
         <v>43444</v>
       </c>
       <c r="B1280">
         <v>2637.72</v>
       </c>
-    </row>
-    <row r="1281" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1280">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1281" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1281" s="2">
         <v>43441</v>
       </c>
       <c r="B1281">
         <v>2633.08</v>
       </c>
-    </row>
-    <row r="1282" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1281">
+        <v>1</v>
+      </c>
+      <c r="D1281">
+        <f>(B1281-$B$1282)/$B$1282</f>
+        <v>-2.3320165433335149E-2</v>
+      </c>
+    </row>
+    <row r="1282" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1282" s="2">
         <v>43440</v>
       </c>
       <c r="B1282">
         <v>2695.95</v>
       </c>
-    </row>
-    <row r="1283" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1282">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1283" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1283" s="2">
         <v>43438</v>
       </c>
@@ -10694,7 +10816,7 @@
         <v>2700.06</v>
       </c>
     </row>
-    <row r="1284" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1284" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1284" s="2">
         <v>43437</v>
       </c>
@@ -10702,7 +10824,7 @@
         <v>2790.37</v>
       </c>
     </row>
-    <row r="1285" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1285" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1285" s="2">
         <v>43434</v>
       </c>
@@ -10710,7 +10832,7 @@
         <v>2760.17</v>
       </c>
     </row>
-    <row r="1286" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1286" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1286" s="2">
         <v>43433</v>
       </c>
@@ -10718,7 +10840,7 @@
         <v>2737.76</v>
       </c>
     </row>
-    <row r="1287" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1287" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1287" s="2">
         <v>43432</v>
       </c>
@@ -10726,7 +10848,7 @@
         <v>2743.79</v>
       </c>
     </row>
-    <row r="1288" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1288" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1288" s="2">
         <v>43431</v>
       </c>
@@ -10734,7 +10856,7 @@
         <v>2682.17</v>
       </c>
     </row>
-    <row r="1289" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1289" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1289" s="2">
         <v>43430</v>
       </c>
@@ -10742,7 +10864,7 @@
         <v>2673.45</v>
       </c>
     </row>
-    <row r="1290" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1290" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1290" s="2">
         <v>43427</v>
       </c>
@@ -10750,7 +10872,7 @@
         <v>2632.56</v>
       </c>
     </row>
-    <row r="1291" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1291" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1291" s="2">
         <v>43425</v>
       </c>
@@ -10758,7 +10880,7 @@
         <v>2649.93</v>
       </c>
     </row>
-    <row r="1292" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1292" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1292" s="2">
         <v>43424</v>
       </c>
@@ -10766,7 +10888,7 @@
         <v>2641.89</v>
       </c>
     </row>
-    <row r="1293" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1293" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1293" s="2">
         <v>43423</v>
       </c>
@@ -10774,7 +10896,7 @@
         <v>2690.73</v>
       </c>
     </row>
-    <row r="1294" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1294" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1294" s="2">
         <v>43420</v>
       </c>
@@ -10782,7 +10904,7 @@
         <v>2736.27</v>
       </c>
     </row>
-    <row r="1295" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1295" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1295" s="2">
         <v>43419</v>
       </c>
@@ -10790,7 +10912,7 @@
         <v>2730.2</v>
       </c>
     </row>
-    <row r="1296" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1296" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1296" s="2">
         <v>43418</v>
       </c>
@@ -22318,7 +22440,7 @@
         <v>1514.68</v>
       </c>
     </row>
-    <row r="2737" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2737" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2737" s="2">
         <v>41332</v>
       </c>
@@ -22326,7 +22448,7 @@
         <v>1515.99</v>
       </c>
     </row>
-    <row r="2738" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2738" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2738" s="2">
         <v>41331</v>
       </c>
@@ -22334,7 +22456,7 @@
         <v>1496.94</v>
       </c>
     </row>
-    <row r="2739" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2739" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2739" s="2">
         <v>41330</v>
       </c>
@@ -22342,7 +22464,7 @@
         <v>1487.85</v>
       </c>
     </row>
-    <row r="2740" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2740" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2740" s="2">
         <v>41327</v>
       </c>
@@ -22350,7 +22472,7 @@
         <v>1515.6</v>
       </c>
     </row>
-    <row r="2741" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2741" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2741" s="2">
         <v>41326</v>
       </c>
@@ -22358,7 +22480,7 @@
         <v>1502.42</v>
       </c>
     </row>
-    <row r="2742" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2742" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2742" s="2">
         <v>41325</v>
       </c>
@@ -22366,7 +22488,7 @@
         <v>1511.95</v>
       </c>
     </row>
-    <row r="2743" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2743" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2743" s="2">
         <v>41324</v>
       </c>
@@ -22374,7 +22496,7 @@
         <v>1530.94</v>
       </c>
     </row>
-    <row r="2744" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2744" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2744" s="2">
         <v>41320</v>
       </c>
@@ -22382,7 +22504,7 @@
         <v>1519.79</v>
       </c>
     </row>
-    <row r="2745" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2745" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2745" s="2">
         <v>41319</v>
       </c>
@@ -22390,7 +22512,7 @@
         <v>1521.38</v>
       </c>
     </row>
-    <row r="2746" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2746" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2746" s="2">
         <v>41318</v>
       </c>
@@ -22398,7 +22520,7 @@
         <v>1520.33</v>
       </c>
     </row>
-    <row r="2747" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2747" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2747" s="2">
         <v>41317</v>
       </c>
@@ -22406,7 +22528,7 @@
         <v>1519.43</v>
       </c>
     </row>
-    <row r="2748" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2748" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2748" s="2">
         <v>41316</v>
       </c>
@@ -22414,7 +22536,7 @@
         <v>1517.01</v>
       </c>
     </row>
-    <row r="2749" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2749" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2749" s="2">
         <v>41313</v>
       </c>
@@ -22422,7 +22544,7 @@
         <v>1517.93</v>
       </c>
     </row>
-    <row r="2750" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2750" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2750" s="2">
         <v>41312</v>
       </c>
@@ -22430,119 +22552,177 @@
         <v>1509.39</v>
       </c>
     </row>
-    <row r="2751" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2751" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2751" s="2">
         <v>41311</v>
       </c>
       <c r="B2751">
         <v>1512.12</v>
       </c>
-    </row>
-    <row r="2752" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2751">
+        <v>14</v>
+      </c>
+      <c r="D2751">
+        <f>(B2751-$B$2765)/$B$2765</f>
+        <v>2.6815968709044211E-2</v>
+      </c>
+    </row>
+    <row r="2752" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2752" s="2">
         <v>41310</v>
       </c>
       <c r="B2752">
         <v>1511.29</v>
       </c>
-    </row>
-    <row r="2753" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2752">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2753" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2753" s="2">
         <v>41309</v>
       </c>
       <c r="B2753">
         <v>1495.71</v>
       </c>
-    </row>
-    <row r="2754" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2753">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2754" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2754" s="2">
         <v>41306</v>
       </c>
       <c r="B2754">
         <v>1513.17</v>
       </c>
-    </row>
-    <row r="2755" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2754">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2755" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2755" s="2">
         <v>41305</v>
       </c>
       <c r="B2755">
         <v>1498.11</v>
       </c>
-    </row>
-    <row r="2756" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2755">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2756" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2756" s="2">
         <v>41304</v>
       </c>
       <c r="B2756">
         <v>1501.96</v>
       </c>
-    </row>
-    <row r="2757" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2756">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2757" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2757" s="2">
         <v>41303</v>
       </c>
       <c r="B2757">
         <v>1507.84</v>
       </c>
-    </row>
-    <row r="2758" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2757">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2758" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2758" s="2">
         <v>41302</v>
       </c>
       <c r="B2758">
         <v>1500.18</v>
       </c>
-    </row>
-    <row r="2759" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2758">
+        <v>7</v>
+      </c>
+      <c r="D2758">
+        <f>(B2758-$B$2765)/$B$2765</f>
+        <v>1.8708025777011167E-2</v>
+      </c>
+    </row>
+    <row r="2759" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2759" s="2">
         <v>41299</v>
       </c>
       <c r="B2759">
         <v>1502.96</v>
       </c>
-    </row>
-    <row r="2760" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2759">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2760" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2760" s="2">
         <v>41298</v>
       </c>
       <c r="B2760">
         <v>1494.82</v>
       </c>
-    </row>
-    <row r="2761" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2760">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2761" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2761" s="2">
         <v>41297</v>
       </c>
       <c r="B2761">
         <v>1494.81</v>
       </c>
-    </row>
-    <row r="2762" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2761">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2762" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2762" s="2">
         <v>41296</v>
       </c>
       <c r="B2762">
         <v>1492.56</v>
       </c>
-    </row>
-    <row r="2763" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2762">
+        <v>3</v>
+      </c>
+      <c r="D2762">
+        <f>(B2762-$B$2765)/$B$2765</f>
+        <v>1.3533609935964794E-2</v>
+      </c>
+    </row>
+    <row r="2763" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2763" s="2">
         <v>41292</v>
       </c>
       <c r="B2763">
         <v>1485.98</v>
       </c>
-    </row>
-    <row r="2764" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2763">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2764" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2764" s="2">
         <v>41291</v>
       </c>
       <c r="B2764">
         <v>1480.94</v>
       </c>
-    </row>
-    <row r="2765" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2764">
+        <v>1</v>
+      </c>
+      <c r="D2764">
+        <f>(B2764-$B$2765)/$B$2765</f>
+        <v>5.6429653069677687E-3</v>
+      </c>
+    </row>
+    <row r="2765" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2765" s="2">
         <v>41290</v>
       </c>
@@ -22550,7 +22730,7 @@
         <v>1472.63</v>
       </c>
     </row>
-    <row r="2766" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2766" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2766" s="2">
         <v>41289</v>
       </c>
@@ -22558,7 +22738,7 @@
         <v>1472.34</v>
       </c>
     </row>
-    <row r="2767" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2767" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2767" s="2">
         <v>41288</v>
       </c>
@@ -22566,7 +22746,7 @@
         <v>1470.68</v>
       </c>
     </row>
-    <row r="2768" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2768" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2768" s="2">
         <v>41285</v>
       </c>

</xml_diff>